<commit_message>
Fix variablechange to use self instead of local variables
</commit_message>
<xml_diff>
--- a/Conversion Technologies Database.xlsx
+++ b/Conversion Technologies Database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/albertrehnberg/Desktop/projekt/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86F4D768-0CF4-C14C-BD42-527CB1F39CF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15DAAB81-02AD-C545-9D1D-8E65B696124B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Solar PV" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="62">
   <si>
     <t>Name</t>
   </si>
@@ -132,9 +132,6 @@
   </si>
   <si>
     <t>KIT SOLAR TERMOSSIFÃO 300 LTS</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 1 968.00</t>
   </si>
   <si>
     <t>https://arcalda.com/paineis-solares/2343-kit-solar-termossifao-200-lts.html?gclid=Cj0KCQjw5JSLBhCxARIsAHgO2ScWqLN9mnbnyY9yrZrfpBGkfsM6-WVT5PoLaPfDDl06vEtXMvv92XwaAnenEALw_wcB</t>
@@ -674,8 +671,8 @@
   </sheetPr>
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -686,7 +683,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" customHeight="1">
       <c r="A1" s="23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -724,7 +721,7 @@
         <v>0.2</v>
       </c>
       <c r="F2" s="3">
-        <v>179.69</v>
+        <v>180</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>8</v>
@@ -816,7 +813,7 @@
         <v>0.2</v>
       </c>
       <c r="F6" s="2">
-        <v>177.7</v>
+        <v>178</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>16</v>
@@ -996,7 +993,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" customHeight="1">
       <c r="A1" s="22" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>0</v>
@@ -1022,7 +1019,7 @@
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1">
       <c r="A2" s="22" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>32</v>
@@ -1039,19 +1036,19 @@
       <c r="F2" s="2">
         <v>1.8</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="10">
+        <v>1968</v>
+      </c>
+      <c r="H2" s="6" t="s">
         <v>33</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15.75" customHeight="1">
       <c r="A3" s="22" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C3" s="2">
         <v>620</v>
@@ -1069,15 +1066,15 @@
         <v>2000</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="15.75" customHeight="1">
       <c r="A4" s="22" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C4">
         <v>100</v>
@@ -1095,15 +1092,15 @@
         <v>1566</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="15.75" customHeight="1">
       <c r="A5" s="22" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C5">
         <v>100</v>
@@ -1118,19 +1115,18 @@
         <v>2.12</v>
       </c>
       <c r="G5" s="14">
-        <f>999</f>
         <v>999</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="15.75" customHeight="1">
       <c r="A6" s="22" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C6">
         <v>100</v>
@@ -1148,15 +1144,15 @@
         <v>2047.38</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="15.75" customHeight="1">
       <c r="A7" s="22" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C7">
         <v>100</v>
@@ -1174,7 +1170,7 @@
         <v>2654.65</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -1197,7 +1193,7 @@
   </sheetPr>
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
@@ -1208,7 +1204,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" customHeight="1">
       <c r="A1" s="22" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1217,24 +1213,24 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>46</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15.75" customHeight="1">
       <c r="A2" s="22" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C2" s="2">
         <v>3000</v>
@@ -1249,15 +1245,15 @@
         <v>700</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.75" customHeight="1">
       <c r="A3" s="22" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C3" s="2">
         <v>2000</v>
@@ -1272,15 +1268,15 @@
         <v>690</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="15.75" customHeight="1">
       <c r="A4" s="22" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C4" s="2">
         <v>600</v>
@@ -1295,15 +1291,15 @@
         <v>859</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="15.75" customHeight="1">
       <c r="A5" s="22" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C5" s="2">
         <v>940</v>
@@ -1318,15 +1314,15 @@
         <v>480</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="15.75" customHeight="1">
       <c r="A6" s="22" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C6" s="2">
         <v>10000</v>
@@ -1341,15 +1337,15 @@
         <v>3000</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="15.75" customHeight="1">
       <c r="A7" s="22" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C7" s="2">
         <v>1500</v>
@@ -1364,7 +1360,7 @@
         <v>1199</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>